<commit_message>
simple serch feature ready and fix filtered search
</commit_message>
<xml_diff>
--- a/public/Vladimirputine.xlsx
+++ b/public/Vladimirputine.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="37">
   <si>
     <t>Search Input</t>
   </si>
@@ -37,7 +37,7 @@
     <t>Style</t>
   </si>
   <si>
-    <t>Vladimir putine</t>
+    <t>vladimir putine</t>
   </si>
   <si>
     <t>Potential match detected</t>
@@ -67,10 +67,61 @@
     <t>todoByFrontDev/655170123456789012345678</t>
   </si>
   <si>
-    <t>2. (86.75%) -  Vladimir Vladimirovich Putin</t>
+    <t>2. (100%) -  Vladimir Vladimirovich Putin</t>
+  </si>
+  <si>
+    <t>US - Liste OFAC des ressortissants spécialement désignés et des personnes bloquées (SDN)</t>
+  </si>
+  <si>
+    <t>todoByFrontDev/975901234567890123456789</t>
+  </si>
+  <si>
+    <t>3. (98.65%) -  Vladimir Vladimirovich Poutine</t>
+  </si>
+  <si>
+    <t>FR - Liste de sanctions de la Direction Générale du Trésor (DGT)</t>
+  </si>
+  <si>
+    <t>todoByFrontDev/713310123456789012345678</t>
+  </si>
+  <si>
+    <t>4. (95.84%) -  Vladimir Vladimirovich Putin</t>
+  </si>
+  <si>
+    <t>5. (95.84%) -  Vladimir Vladimirovich Putin</t>
+  </si>
+  <si>
+    <t>CA - Liste consolidée des sanctions autonomes canadiennes</t>
+  </si>
+  <si>
+    <t>1952</t>
+  </si>
+  <si>
+    <t>todoByFrontDev/742020123456789012345678</t>
+  </si>
+  <si>
+    <t>6. (89.69%) -  Vladimir Vladimirovich Putin</t>
+  </si>
+  <si>
+    <t>UE - Liste consolidée des personnes, groupes et entités faisant l'objet de sanctions financières de l'UE</t>
+  </si>
+  <si>
+    <t>todoByFrontDev/171350123456789012345678</t>
+  </si>
+  <si>
+    <t>7. (86.75%) -  Vladimir Vladimirovich Putin</t>
   </si>
   <si>
     <t>todoByFrontDev/655190123456789012345678</t>
+  </si>
+  <si>
+    <t>8. (83.9%) -  Vladimir Vladimirovich Putin</t>
+  </si>
+  <si>
+    <t>9. (82.08%) -  Vladimir Vladimirovich Putin</t>
+  </si>
+  <si>
+    <t>10. (82.08%) -  Vladimir Vladimirovich Putin</t>
   </si>
 </sst>
 </file>
@@ -523,7 +574,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H13"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
@@ -630,7 +681,7 @@
         <v>18</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>13</v>
@@ -640,9 +691,185 @@
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="B6" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="9"/>
+      <c r="G6" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="3">
+      <c r="D7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="9"/>
+      <c r="G7" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="9"/>
+      <c r="G8" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
+      <c r="B9" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="9"/>
+      <c r="G9" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
+      <c r="B10" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="9"/>
+      <c r="G10" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="9"/>
+      <c r="G11" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="9"/>
+      <c r="G12" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H12" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+      <c r="B13" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="9"/>
+      <c r="G13" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H13" s="3">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
search feature ok and tested
</commit_message>
<xml_diff>
--- a/public/Vladimirputine.xlsx
+++ b/public/Vladimirputine.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
     <t>Search Input</t>
   </si>
@@ -37,7 +37,7 @@
     <t>Style</t>
   </si>
   <si>
-    <t>vladimir putine</t>
+    <t>Vladimir putine</t>
   </si>
   <si>
     <t>Potential match detected</t>
@@ -67,7 +67,7 @@
     <t>todoByFrontDev/655170123456789012345678</t>
   </si>
   <si>
-    <t>2. (100%) -  Vladimir Vladimirovich Putin</t>
+    <t>2. (95.84%) -  Vladimir Vladimirovich Putin</t>
   </si>
   <si>
     <t>US - Liste OFAC des ressortissants spécialement désignés et des personnes bloquées (SDN)</t>
@@ -76,52 +76,10 @@
     <t>todoByFrontDev/975901234567890123456789</t>
   </si>
   <si>
-    <t>3. (98.65%) -  Vladimir Vladimirovich Poutine</t>
-  </si>
-  <si>
-    <t>FR - Liste de sanctions de la Direction Générale du Trésor (DGT)</t>
-  </si>
-  <si>
-    <t>todoByFrontDev/713310123456789012345678</t>
-  </si>
-  <si>
-    <t>4. (95.84%) -  Vladimir Vladimirovich Putin</t>
-  </si>
-  <si>
-    <t>5. (95.84%) -  Vladimir Vladimirovich Putin</t>
-  </si>
-  <si>
-    <t>CA - Liste consolidée des sanctions autonomes canadiennes</t>
-  </si>
-  <si>
-    <t>1952</t>
-  </si>
-  <si>
-    <t>todoByFrontDev/742020123456789012345678</t>
-  </si>
-  <si>
-    <t>6. (89.69%) -  Vladimir Vladimirovich Putin</t>
-  </si>
-  <si>
-    <t>UE - Liste consolidée des personnes, groupes et entités faisant l'objet de sanctions financières de l'UE</t>
-  </si>
-  <si>
-    <t>todoByFrontDev/171350123456789012345678</t>
-  </si>
-  <si>
-    <t>7. (86.75%) -  Vladimir Vladimirovich Putin</t>
+    <t>3. (86.75%) -  Vladimir Vladimirovich Putin</t>
   </si>
   <si>
     <t>todoByFrontDev/655190123456789012345678</t>
-  </si>
-  <si>
-    <t>8. (83.9%) -  Vladimir Vladimirovich Putin</t>
-  </si>
-  <si>
-    <t>9. (82.08%) -  Vladimir Vladimirovich Putin</t>
-  </si>
-  <si>
-    <t>10. (82.08%) -  Vladimir Vladimirovich Putin</t>
   </si>
 </sst>
 </file>
@@ -574,7 +532,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H6"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
@@ -703,7 +661,7 @@
         <v>21</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>13</v>
@@ -713,163 +671,9 @@
       </c>
       <c r="F6" s="9"/>
       <c r="G6" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H6" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="9"/>
-      <c r="G7" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="H8" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="9"/>
-      <c r="G9" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="H9" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="9"/>
-      <c r="G10" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="H10" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="9"/>
-      <c r="G11" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="H11" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" s="9"/>
-      <c r="G12" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="H12" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" s="9"/>
-      <c r="G13" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="H13" s="3">
         <v>3</v>
       </c>
     </row>

</xml_diff>